<commit_message>
Lean localization + Saving + Audio Manager + audio master data to definition(auto-find audio from path)
</commit_message>
<xml_diff>
--- a/Assets/Data/Excel/MasterItem.xlsx
+++ b/Assets/Data/Excel/MasterItem.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_VincentGame\HorrorGame\Assets\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_VincentGame\HorrorGame\Assets\Data\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C9F73BE-ED0A-45B2-B45F-A8648C5B1685}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFC5712A-21A3-4DE7-B9CB-9340B64920B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{CE5CDD7E-8CFD-476C-AB84-63CE99224655}"/>
   </bookViews>
   <sheets>
-    <sheet name="ItemList" sheetId="1" r:id="rId1"/>
+    <sheet name="Entities" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -421,7 +421,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Now able to rotate items within the ui + also correctly updates the title and description for items (still need to check for the pool on return)
</commit_message>
<xml_diff>
--- a/Assets/Data/Excel/MasterItem.xlsx
+++ b/Assets/Data/Excel/MasterItem.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_VincentGame\HorrorGame\Assets\Data\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8D6B0E9-BC9D-4629-9C79-971EE52C44E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4A5016A-210F-473D-B104-A7EC48193A2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{CE5CDD7E-8CFD-476C-AB84-63CE99224655}"/>
   </bookViews>
@@ -457,7 +457,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Changed the way of item localization
</commit_message>
<xml_diff>
--- a/Assets/Data/Excel/MasterItem.xlsx
+++ b/Assets/Data/Excel/MasterItem.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_VincentGame\HorrorGame\Assets\Data\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F756ABCA-6167-417A-A885-DEBAC3B2841F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD3EF106-63FB-410A-B577-AF80E4B9E882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{CE5CDD7E-8CFD-476C-AB84-63CE99224655}"/>
   </bookViews>
@@ -34,14 +34,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>id</t>
   </si>
   <si>
-    <t>name</t>
-  </si>
-  <si>
     <t>Item_1</t>
   </si>
   <si>
@@ -63,20 +60,23 @@
     <t>Item_Key_A</t>
   </si>
   <si>
-    <t>Old Key</t>
-  </si>
-  <si>
-    <t>Puzzle Piece A</t>
-  </si>
-  <si>
-    <t>Puzzle Piece B</t>
+    <t>Item_Book_A</t>
+  </si>
+  <si>
+    <t>Item_Book_B</t>
+  </si>
+  <si>
+    <t>Item_Book_C</t>
+  </si>
+  <si>
+    <t>key</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -91,8 +91,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -102,6 +116,16 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -129,15 +153,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="1" builtinId="10"/>
   </cellStyles>
@@ -451,18 +481,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94E91137-7BD2-48ED-A93D-3ECC6F638E0D}">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.6640625" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" customWidth="1"/>
-    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="39.77734375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -471,71 +503,105 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2">
+        <v>10001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="C4" s="3">
+        <v>10100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" s="3">
+        <v>10101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="2">
+        <v>10201</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="3">
+        <v>10301</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="3">
+        <v>10302</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" t="s">
-        <v>9</v>
+      <c r="C9" s="3">
+        <v>10303</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Removed the speed parameter from player's animator + State restructure + script name changed + MasterQuest and UI quest show(not really developed) + Event trigger on touch collider
</commit_message>
<xml_diff>
--- a/Assets/Data/Excel/MasterItem.xlsx
+++ b/Assets/Data/Excel/MasterItem.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_VincentGame\HorrorGame\Assets\Data\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD3EF106-63FB-410A-B577-AF80E4B9E882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B92306F-6E29-44BE-995F-14A136B98D24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{CE5CDD7E-8CFD-476C-AB84-63CE99224655}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>id</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>key</t>
+  </si>
+  <si>
+    <t>Coin</t>
   </si>
 </sst>
 </file>
@@ -481,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94E91137-7BD2-48ED-A93D-3ECC6F638E0D}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -600,6 +603,17 @@
         <v>10303</v>
       </c>
     </row>
+    <row r="10" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="3">
+        <v>10304</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>